<commit_message>
fichiers SCRUM et UML
</commit_message>
<xml_diff>
--- a/SCRUM/Template suivi projet Fred-Salah.xlsx
+++ b/SCRUM/Template suivi projet Fred-Salah.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagiaire\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagiaire\Desktop\Nouveau dossier\Proxibanque-V3\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D3C8FFFF-942F-4002-8C40-B4E442D4C77C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A0645E07-686E-4D67-934D-8244B0AD0759}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8805" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8805" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint1 Backlog" sheetId="4" r:id="rId2"/>
-    <sheet name="Story Mapping" sheetId="6" r:id="rId3"/>
+    <sheet name="Story Mapping" sheetId="6" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId2"/>
+    <sheet name="Sprint Backlog" sheetId="4" r:id="rId3"/>
     <sheet name="Road Map" sheetId="5" r:id="rId4"/>
     <sheet name="Suivi Release &amp; Vélocité" sheetId="2" r:id="rId5"/>
     <sheet name="Tableau de bord" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$A$4:$Z$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Product Backlog'!$A$4:$Z$18</definedName>
     <definedName name="RP_Sprint_All">'Suivi Release &amp; Vélocité'!$C$7:$F$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="98">
   <si>
     <t>Suivi Release &amp; Vélocité</t>
   </si>
@@ -139,12 +139,6 @@
   </si>
   <si>
     <t>Fin S5</t>
-  </si>
-  <si>
-    <t>Fin S6</t>
-  </si>
-  <si>
-    <t>Fin S7</t>
   </si>
   <si>
     <t>Terminé</t>
@@ -276,27 +270,6 @@
     <t>Gérer les clients et les comptes</t>
   </si>
   <si>
-    <t>Authentification Conseiller</t>
-  </si>
-  <si>
-    <t>Affichage liste clients</t>
-  </si>
-  <si>
-    <t>Suppression client</t>
-  </si>
-  <si>
-    <t>Ajout client</t>
-  </si>
-  <si>
-    <t>Créer compte</t>
-  </si>
-  <si>
-    <t>Débit/Crédit</t>
-  </si>
-  <si>
-    <t>Virement</t>
-  </si>
-  <si>
     <t>nombre de clients</t>
   </si>
   <si>
@@ -325,6 +298,57 @@
   </si>
   <si>
     <t>Supprimer un client</t>
+  </si>
+  <si>
+    <t>Release 1</t>
+  </si>
+  <si>
+    <t>Fonctionnalités Gérant</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Modifier compte</t>
+  </si>
+  <si>
+    <t>Supprimer compte</t>
+  </si>
+  <si>
+    <t>Modifier client</t>
+  </si>
+  <si>
+    <t>Placement boursier</t>
+  </si>
+  <si>
+    <t>Simulation crédit</t>
+  </si>
+  <si>
+    <t>Audit des comptes de l'agence</t>
+  </si>
+  <si>
+    <t>Release 2</t>
+  </si>
+  <si>
+    <t>Release 3</t>
+  </si>
+  <si>
+    <t>Proxibanque V4</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Afficher comptes d'un client</t>
+  </si>
+  <si>
+    <t>Afficher les comptes d'un client</t>
+  </si>
+  <si>
+    <t>Le conseiller peut sélectionner l'un des clients dont il a la charge et voir la liste de ses comptes</t>
+  </si>
+  <si>
+    <t>Dans l'écran 3 montrant la liste des clients, le conseiller sélectionne un client. L'écran 4 s'affiche, il contient la liste des comptes de ce client.</t>
   </si>
 </sst>
 </file>
@@ -422,7 +446,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,12 +486,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,8 +507,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -579,15 +621,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -941,11 +974,249 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -978,9 +1249,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1020,9 +1288,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1045,15 +1310,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1073,16 +1334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1097,53 +1349,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1151,50 +1367,23 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1208,35 +1397,296 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1329,7 +1779,7 @@
             <c:strRef>
               <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -1348,12 +1798,6 @@
                 <c:pt idx="5">
                   <c:v>Fin S5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Fin S6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Fin S7</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
@@ -1364,7 +1808,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,7 +1848,7 @@
             <c:strRef>
               <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -1423,12 +1867,6 @@
                 <c:pt idx="5">
                   <c:v>Fin S5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Fin S6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Fin S7</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
@@ -1439,16 +1877,16 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.75</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.5</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.25</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1491,7 +1929,7 @@
             <c:strRef>
               <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -1510,12 +1948,6 @@
                 <c:pt idx="5">
                   <c:v>Fin S5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Fin S6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Fin S7</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
@@ -1526,19 +1958,16 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.333333333333332</c:v>
+                  <c:v>133.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.6666666666666661</c:v>
+                  <c:v>66.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-5.6666666666666679</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,7 +2007,7 @@
             <c:strRef>
               <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -1597,12 +2026,6 @@
                 <c:pt idx="5">
                   <c:v>Fin S5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Fin S6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Fin S7</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
@@ -1613,19 +2036,19 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.6</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.199999999999999</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8000000000000007</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4000000000000004</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1809,9 +2232,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Suivi Release &amp; Vélocité'!$C$4:$I$4</c:f>
+              <c:f>'Suivi Release &amp; Vélocité'!$C$4:$F$4</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -1824,36 +2247,15 @@
                 <c:pt idx="3">
                   <c:v>Sprint 4</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Sprint 7</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Suivi Release &amp; Vélocité'!$C$5:$I$5</c:f>
+              <c:f>'Suivi Release &amp; Vélocité'!$C$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
+                <c:ptCount val="4"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2070,6 +2472,114 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E754C71-0CF3-42B4-811E-4B97F35CF7AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>628650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C00902-28F5-463F-969A-21170571A4D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>628650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CBCAB2D-E1DE-4634-8078-F25508B6D03D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2481,6 +2991,262 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F492E24B-972E-44AA-8E1C-43F16CCC63B2}">
+  <dimension ref="A2:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" style="41" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="41" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" style="41" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="41" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="59" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" style="59" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" style="59" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" ht="38.25" customHeight="1">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="93" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="95"/>
+      <c r="N2" s="73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+    </row>
+    <row r="4" spans="2:14" ht="25.5">
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="61"/>
+      <c r="J4" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="61"/>
+      <c r="L4" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="N4" s="62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+    </row>
+    <row r="6" spans="2:14" ht="38.25">
+      <c r="B6" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="96" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="58"/>
+      <c r="F6" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="69"/>
+      <c r="H6" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="69"/>
+      <c r="J6" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="69"/>
+      <c r="L6" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+    </row>
+    <row r="7" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="B7" s="100"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+    </row>
+    <row r="8" spans="2:14" ht="25.5">
+      <c r="B8" s="100"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="69"/>
+      <c r="J8" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="70"/>
+      <c r="L8" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+    </row>
+    <row r="9" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="B9" s="100"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+    </row>
+    <row r="10" spans="2:14" ht="25.5">
+      <c r="B10" s="101"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="71"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+    </row>
+    <row r="11" spans="2:14" ht="5.0999999999999996" customHeight="1">
+      <c r="B11" s="72"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="58"/>
+    </row>
+    <row r="12" spans="2:14" ht="25.5">
+      <c r="B12" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="58"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="70"/>
+      <c r="J12" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="70"/>
+      <c r="L12" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="M12" s="77"/>
+      <c r="N12" s="75"/>
+    </row>
+    <row r="13" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="B13" s="100"/>
+      <c r="D13" s="80"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
+    </row>
+    <row r="14" spans="2:14" ht="38.25">
+      <c r="B14" s="101"/>
+      <c r="D14" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="77"/>
+      <c r="L14" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="77"/>
+      <c r="N14" s="76" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B12:B14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2488,7 +3254,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C11"/>
+      <selection activeCell="C5" sqref="C5:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2536,15 +3302,15 @@
     </row>
     <row r="2" spans="1:26" ht="24" customHeight="1">
       <c r="A2" s="4"/>
-      <c r="B2" s="45" t="s">
-        <v>56</v>
+      <c r="B2" s="102" t="s">
+        <v>54</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2576,11 +3342,11 @@
       <c r="H3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <f>SUM(F5:F18)</f>
-        <v>170</v>
+        <v>200</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="6"/>
@@ -2601,29 +3367,29 @@
       <c r="Z3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="6"/>
@@ -2645,29 +3411,29 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="45" customHeight="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="20">
+      <c r="A5" s="16"/>
+      <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>57</v>
+      <c r="C5" s="42" t="s">
+        <v>55</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>37</v>
+      <c r="D5" s="43" t="s">
+        <v>35</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>100</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="19">
         <v>20</v>
       </c>
-      <c r="G5" s="49" t="s">
-        <v>48</v>
+      <c r="G5" s="42" t="s">
+        <v>46</v>
       </c>
-      <c r="H5" s="49" t="s">
-        <v>38</v>
+      <c r="H5" s="42" t="s">
+        <v>36</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="I5" s="44" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="6"/>
@@ -2689,27 +3455,27 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" ht="45" customHeight="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="20">
+      <c r="A6" s="30"/>
+      <c r="B6" s="19">
         <v>2</v>
       </c>
-      <c r="C6" s="49" t="s">
-        <v>43</v>
+      <c r="C6" s="42" t="s">
+        <v>41</v>
       </c>
-      <c r="D6" s="49" t="s">
-        <v>44</v>
+      <c r="D6" s="42" t="s">
+        <v>42</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="33">
         <v>100</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="33">
         <v>30</v>
       </c>
-      <c r="G6" s="52" t="s">
-        <v>51</v>
+      <c r="G6" s="45" t="s">
+        <v>49</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="51" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="44" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="6"/>
@@ -2731,27 +3497,27 @@
       <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="45" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="20">
+      <c r="A7" s="16"/>
+      <c r="B7" s="19">
         <v>3</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>45</v>
+      <c r="C7" s="43" t="s">
+        <v>43</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>46</v>
+      <c r="D7" s="43" t="s">
+        <v>44</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="19">
         <v>40</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="19">
         <v>10</v>
       </c>
-      <c r="G7" s="50" t="s">
-        <v>52</v>
+      <c r="G7" s="43" t="s">
+        <v>50</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="51" t="s">
+      <c r="H7" s="23"/>
+      <c r="I7" s="44" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="6"/>
@@ -2773,27 +3539,27 @@
       <c r="Z7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="45" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="20">
+      <c r="A8" s="16"/>
+      <c r="B8" s="19">
         <v>4</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>35</v>
+      <c r="C8" s="42" t="s">
+        <v>33</v>
       </c>
-      <c r="D8" s="50" t="s">
-        <v>47</v>
+      <c r="D8" s="43" t="s">
+        <v>45</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>40</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>20</v>
       </c>
-      <c r="G8" s="49" t="s">
-        <v>36</v>
+      <c r="G8" s="42" t="s">
+        <v>34</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="27" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="6"/>
@@ -2815,27 +3581,27 @@
       <c r="Z8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="45" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="20">
+      <c r="A9" s="16"/>
+      <c r="B9" s="19">
         <v>5</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>39</v>
+      <c r="C9" s="118" t="s">
+        <v>95</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="119" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="24">
         <v>40</v>
       </c>
-      <c r="E9" s="25">
-        <v>40</v>
-      </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>30</v>
       </c>
-      <c r="G9" s="49" t="s">
-        <v>49</v>
+      <c r="G9" s="118" t="s">
+        <v>97</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="51" t="s">
+      <c r="H9" s="28"/>
+      <c r="I9" s="120" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="6"/>
@@ -2857,27 +3623,27 @@
       <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="45" customHeight="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="20">
+      <c r="A10" s="16"/>
+      <c r="B10" s="19">
         <v>6</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>41</v>
+      <c r="C10" s="42" t="s">
+        <v>37</v>
       </c>
-      <c r="D10" s="49" t="s">
-        <v>42</v>
+      <c r="D10" s="42" t="s">
+        <v>38</v>
       </c>
-      <c r="E10" s="36">
-        <v>20</v>
+      <c r="E10" s="24">
+        <v>40</v>
       </c>
-      <c r="F10" s="36">
-        <v>20</v>
+      <c r="F10" s="24">
+        <v>30</v>
       </c>
-      <c r="G10" s="49" t="s">
-        <v>50</v>
+      <c r="G10" s="42" t="s">
+        <v>47</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="51" t="s">
+      <c r="H10" s="28"/>
+      <c r="I10" s="44" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="6"/>
@@ -2899,27 +3665,27 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="45" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="24">
         <v>7</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>53</v>
+      <c r="C11" s="42" t="s">
+        <v>39</v>
       </c>
-      <c r="D11" s="50" t="s">
-        <v>54</v>
+      <c r="D11" s="42" t="s">
+        <v>40</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="33">
         <v>20</v>
       </c>
-      <c r="F11" s="20">
-        <v>40</v>
+      <c r="F11" s="33">
+        <v>20</v>
       </c>
-      <c r="G11" s="49" t="s">
-        <v>55</v>
+      <c r="G11" s="42" t="s">
+        <v>48</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="51" t="s">
+      <c r="H11" s="34"/>
+      <c r="I11" s="44" t="s">
         <v>20</v>
       </c>
       <c r="J11" s="6"/>
@@ -2941,15 +3707,29 @@
       <c r="Z11" s="6"/>
     </row>
     <row r="12" spans="1:26" ht="45" customHeight="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="27"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="19">
+        <v>8</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="24">
+        <v>20</v>
+      </c>
+      <c r="F12" s="19">
+        <v>40</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="44" t="s">
+        <v>20</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -2969,15 +3749,15 @@
       <c r="Z12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="34.5" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="27"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -2997,15 +3777,15 @@
       <c r="Z13" s="6"/>
     </row>
     <row r="14" spans="1:26" ht="45" customHeight="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="27"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -3026,14 +3806,14 @@
     </row>
     <row r="15" spans="1:26" ht="56.25" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="27"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="25"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -3054,14 +3834,14 @@
     </row>
     <row r="16" spans="1:26" ht="56.25" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="27"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="25"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -3082,14 +3862,14 @@
     </row>
     <row r="17" spans="1:26" ht="56.25" customHeight="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="27"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="25"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -3110,14 +3890,14 @@
     </row>
     <row r="18" spans="1:26" ht="56.25" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="27"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="25"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -3141,7 +3921,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="40"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -3169,7 +3949,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="40"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -3197,7 +3977,7 @@
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="40"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -3225,7 +4005,7 @@
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="40"/>
+      <c r="E22" s="36"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -3253,7 +4033,7 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="40"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -3281,7 +4061,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="40"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -30593,509 +31373,1028 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DDBCDC-F765-4DDA-9FE4-09EDBA49ADF4}">
-  <dimension ref="B1:F23"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B20"/>
+      <selection activeCell="B4" sqref="B4:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="40" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="65" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="13.5" thickBot="1"/>
-    <row r="2" spans="2:6" ht="13.5" thickBot="1">
-      <c r="B2" s="69" t="s">
-        <v>64</v>
+    <row r="1" spans="1:15" s="65" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A1" s="65">
+        <v>16</v>
       </c>
-      <c r="C2" s="70" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="13.5" thickBot="1">
+      <c r="C2" s="115" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="117"/>
+      <c r="J2" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="117"/>
+      <c r="L2" s="116" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="117"/>
+      <c r="N2" s="116" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="117"/>
+    </row>
+    <row r="3" spans="1:15" ht="13.5" thickBot="1">
+      <c r="B3" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="71" t="s">
+      <c r="F3" s="50" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="15" customHeight="1">
-      <c r="B3" s="57" t="s">
+      <c r="G3" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="129" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="130" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="129" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="130" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="129" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="130" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="129" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="130" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1">
+      <c r="B4" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="140">
+        <v>20</v>
+      </c>
+      <c r="D4" s="104">
+        <f>A$1*C4/'Product Backlog'!I$3</f>
+        <v>1.6</v>
+      </c>
+      <c r="E4" s="104">
+        <f>60*D4</f>
+        <v>96</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="46">
+        <v>15</v>
+      </c>
+      <c r="H4" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="144">
+        <v>15</v>
+      </c>
+      <c r="J4" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="125"/>
+      <c r="L4" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="125"/>
+      <c r="N4" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="125"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1">
+      <c r="B5" s="132"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="58">
+      <c r="G5" s="47">
+        <v>66</v>
+      </c>
+      <c r="H5" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="126">
+        <v>60</v>
+      </c>
+      <c r="J5" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="145">
+        <v>6</v>
+      </c>
+      <c r="L5" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="126"/>
+      <c r="N5" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="126"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B6" s="133"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="48">
+        <v>15</v>
+      </c>
+      <c r="H6" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="128"/>
+      <c r="J6" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="128"/>
+      <c r="L6" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="128"/>
+      <c r="N6" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1">
+      <c r="B7" s="131" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="140">
+        <v>30</v>
+      </c>
+      <c r="D7" s="104">
+        <f>A$1*C7/'Product Backlog'!I$3</f>
+        <v>2.4</v>
+      </c>
+      <c r="E7" s="104">
+        <f t="shared" ref="E7" si="0">60*D7</f>
+        <v>144</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="46">
+        <v>15</v>
+      </c>
+      <c r="H7" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="144">
+        <v>15</v>
+      </c>
+      <c r="J7" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="125"/>
+      <c r="L7" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="125"/>
+      <c r="N7" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="125"/>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1">
+      <c r="B8" s="132"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="47">
+        <v>114</v>
+      </c>
+      <c r="H8" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="126">
+        <v>60</v>
+      </c>
+      <c r="J8" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="145">
+        <v>54</v>
+      </c>
+      <c r="L8" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="126"/>
+      <c r="N8" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" s="126"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B9" s="133"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="48">
+        <v>15</v>
+      </c>
+      <c r="H9" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="128"/>
+      <c r="J9" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="128"/>
+      <c r="L9" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="128"/>
+      <c r="N9" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1">
+      <c r="B10" s="131" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="140">
+        <v>10</v>
+      </c>
+      <c r="D10" s="104">
+        <f>A$1*C10/'Product Backlog'!I$3</f>
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="104">
+        <f t="shared" ref="E10" si="1">60*D10</f>
+        <v>48</v>
+      </c>
+      <c r="F10" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="46">
+        <v>15</v>
+      </c>
+      <c r="H10" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="144">
+        <v>15</v>
+      </c>
+      <c r="J10" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="125"/>
+      <c r="L10" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="125"/>
+      <c r="N10" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="125"/>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1">
+      <c r="B11" s="132"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="47">
+        <v>18</v>
+      </c>
+      <c r="H11" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="126"/>
+      <c r="J11" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="145">
+        <v>18</v>
+      </c>
+      <c r="L11" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" s="126"/>
+      <c r="N11" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" s="126"/>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B12" s="133"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="48">
+        <v>15</v>
+      </c>
+      <c r="H12" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="128"/>
+      <c r="J12" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="128"/>
+      <c r="L12" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="128"/>
+      <c r="N12" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" s="146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1">
+      <c r="B13" s="131" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="140">
         <v>20</v>
       </c>
-      <c r="D3" s="59">
-        <v>2</v>
+      <c r="D13" s="104">
+        <f>A$1*C13/'Product Backlog'!I$3</f>
+        <v>1.6</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E13" s="104">
+        <f t="shared" ref="E13" si="2">60*D13</f>
+        <v>96</v>
+      </c>
+      <c r="F13" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="46">
+        <v>15</v>
+      </c>
+      <c r="H13" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="144">
+        <v>15</v>
+      </c>
+      <c r="J13" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="125"/>
+      <c r="L13" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" s="125"/>
+      <c r="N13" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="125"/>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1">
+      <c r="B14" s="132"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="47">
+        <v>66</v>
+      </c>
+      <c r="H14" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="126"/>
+      <c r="J14" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="145">
+        <v>66</v>
+      </c>
+      <c r="L14" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M14" s="126"/>
+      <c r="N14" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O14" s="126"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B15" s="133"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="61">
+      <c r="G15" s="48">
+        <v>15</v>
+      </c>
+      <c r="H15" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="128"/>
+      <c r="J15" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="128"/>
+      <c r="L15" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" s="128"/>
+      <c r="N15" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" s="146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1">
+      <c r="B16" s="134" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="140">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="15" customHeight="1">
-      <c r="B4" s="62"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="54" t="s">
-        <v>59</v>
+      <c r="D16" s="104">
+        <f>A$1*C16/'Product Backlog'!I$3</f>
+        <v>2.4</v>
       </c>
-      <c r="F4" s="63">
-        <v>75</v>
+      <c r="E16" s="104">
+        <f t="shared" ref="E16" si="3">60*D16</f>
+        <v>144</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67" t="s">
-        <v>60</v>
+      <c r="F16" s="66" t="s">
+        <v>56</v>
       </c>
-      <c r="F5" s="68">
+      <c r="G16" s="46">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="15" customHeight="1">
-      <c r="B6" s="57" t="s">
-        <v>43</v>
+      <c r="H16" s="137" t="s">
+        <v>56</v>
       </c>
-      <c r="C6" s="58">
+      <c r="I16" s="144">
+        <v>15</v>
+      </c>
+      <c r="J16" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="125"/>
+      <c r="L16" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="125"/>
+      <c r="N16" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O16" s="125"/>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1">
+      <c r="B17" s="135"/>
+      <c r="C17" s="141"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="47">
+        <v>114</v>
+      </c>
+      <c r="H17" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="126"/>
+      <c r="J17" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" s="126">
+        <v>96</v>
+      </c>
+      <c r="L17" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M17" s="145">
+        <v>18</v>
+      </c>
+      <c r="N17" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O17" s="126"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B18" s="136"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="48">
+        <v>15</v>
+      </c>
+      <c r="H18" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="128"/>
+      <c r="J18" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="128"/>
+      <c r="L18" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="128"/>
+      <c r="N18" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O18" s="146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1">
+      <c r="B19" s="131" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="140">
+        <v>20</v>
+      </c>
+      <c r="D19" s="104">
+        <f>A$1*C19/'Product Backlog'!I$3</f>
+        <v>1.6</v>
+      </c>
+      <c r="E19" s="104">
+        <f t="shared" ref="E19" si="4">60*D19</f>
+        <v>96</v>
+      </c>
+      <c r="F19" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="46">
+        <v>15</v>
+      </c>
+      <c r="H19" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="144">
+        <v>15</v>
+      </c>
+      <c r="J19" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="125"/>
+      <c r="L19" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="125"/>
+      <c r="N19" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O19" s="125"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1">
+      <c r="B20" s="132"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="47">
+        <v>66</v>
+      </c>
+      <c r="H20" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="126"/>
+      <c r="J20" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="126"/>
+      <c r="L20" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="145">
+        <v>66</v>
+      </c>
+      <c r="N20" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O20" s="126"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B21" s="133"/>
+      <c r="C21" s="142"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="48">
+        <v>15</v>
+      </c>
+      <c r="H21" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="128"/>
+      <c r="J21" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" s="128"/>
+      <c r="L21" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="128"/>
+      <c r="N21" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O21" s="146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1">
+      <c r="B22" s="131" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="140">
+        <v>40</v>
+      </c>
+      <c r="D22" s="104">
+        <f>A$1*C22/'Product Backlog'!I$3</f>
+        <v>3.2</v>
+      </c>
+      <c r="E22" s="104">
+        <f t="shared" ref="E22" si="5">60*D22</f>
+        <v>192</v>
+      </c>
+      <c r="F22" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="46">
+        <v>15</v>
+      </c>
+      <c r="H22" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="144">
+        <v>15</v>
+      </c>
+      <c r="J22" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="125"/>
+      <c r="L22" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M22" s="125"/>
+      <c r="N22" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O22" s="125"/>
+    </row>
+    <row r="23" spans="1:15" ht="15" customHeight="1">
+      <c r="B23" s="132"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="47">
+        <v>162</v>
+      </c>
+      <c r="H23" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="126"/>
+      <c r="J23" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="126"/>
+      <c r="L23" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" s="126">
+        <v>156</v>
+      </c>
+      <c r="N23" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="145">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B24" s="133"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="106"/>
+      <c r="F24" s="121" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="122">
+        <v>15</v>
+      </c>
+      <c r="H24" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="128"/>
+      <c r="J24" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" s="128"/>
+      <c r="L24" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="M24" s="128"/>
+      <c r="N24" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O24" s="146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1">
+      <c r="B25" s="148" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="140">
         <v>30</v>
       </c>
-      <c r="D6" s="59">
-        <v>3</v>
+      <c r="D25" s="124">
+        <f>A$1*C25/'Product Backlog'!I$3</f>
+        <v>2.4</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E25" s="104">
+        <f t="shared" ref="E25" si="6">60*D25</f>
+        <v>144</v>
+      </c>
+      <c r="F25" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="46">
+        <v>15</v>
+      </c>
+      <c r="H25" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="144">
+        <v>15</v>
+      </c>
+      <c r="J25" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="125"/>
+      <c r="L25" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="125"/>
+      <c r="N25" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="O25" s="125"/>
+    </row>
+    <row r="26" spans="1:15" ht="15" customHeight="1">
+      <c r="B26" s="149"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="47">
+        <v>114</v>
+      </c>
+      <c r="H26" s="138" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="126"/>
+      <c r="J26" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K26" s="126"/>
+      <c r="L26" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="M26" s="126"/>
+      <c r="N26" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="O26" s="145">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" thickBot="1">
+      <c r="B27" s="150"/>
+      <c r="C27" s="142"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="61">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1">
-      <c r="B7" s="62"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="63">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B8" s="64"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="68">
+      <c r="G27" s="48">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="15" customHeight="1">
-      <c r="B9" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="58">
-        <v>10</v>
-      </c>
-      <c r="D9" s="59">
-        <v>1</v>
-      </c>
-      <c r="E9" s="60" t="s">
+      <c r="H27" s="139" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="61">
-        <v>30</v>
+      <c r="I27" s="128"/>
+      <c r="J27" s="68" t="s">
+        <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1">
-      <c r="B10" s="62"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="54" t="s">
-        <v>59</v>
+      <c r="K27" s="128"/>
+      <c r="L27" s="68" t="s">
+        <v>58</v>
       </c>
-      <c r="F10" s="63">
+      <c r="M27" s="128"/>
+      <c r="N27" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="O27" s="146">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67" t="s">
-        <v>60</v>
+    <row r="30" spans="1:15">
+      <c r="I30">
+        <f>SUM(I4:I27)</f>
+        <v>240</v>
       </c>
-      <c r="F11" s="68">
-        <v>15</v>
+      <c r="K30" s="65">
+        <f>SUM(K4:K27)</f>
+        <v>240</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="15" customHeight="1">
-      <c r="B12" s="57" t="s">
-        <v>35</v>
+      <c r="M30" s="65">
+        <f>SUM(M4:M27)</f>
+        <v>240</v>
       </c>
-      <c r="C12" s="58">
-        <v>20</v>
+      <c r="O30" s="65">
+        <f>SUM(O4:O27)</f>
+        <v>240</v>
       </c>
-      <c r="D12" s="59">
-        <v>2</v>
-      </c>
-      <c r="E12" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="61">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15" customHeight="1">
-      <c r="B13" s="62"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="63">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="68">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="15" customHeight="1">
-      <c r="B15" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="58">
-        <v>30</v>
-      </c>
-      <c r="D15" s="59">
-        <v>3</v>
-      </c>
-      <c r="E15" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="61">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15" customHeight="1">
-      <c r="B16" s="62"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="63">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="64"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="68">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1">
-      <c r="B18" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="58">
-        <v>20</v>
-      </c>
-      <c r="D18" s="59">
-        <v>2</v>
-      </c>
-      <c r="E18" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="61">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="15" customHeight="1">
-      <c r="B19" s="62"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="63">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="68">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="15" customHeight="1">
-      <c r="B21" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="58">
-        <v>40</v>
-      </c>
-      <c r="D21" s="59">
-        <v>4</v>
-      </c>
-      <c r="E21" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="61">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15" customHeight="1">
-      <c r="B22" s="62"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="63">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15" customHeight="1" thickBot="1">
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="68">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="58"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="58"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="58"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="58"/>
+      <c r="B33" s="147"/>
+      <c r="C33" s="58"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="58"/>
+      <c r="B34" s="147"/>
+      <c r="C34" s="58"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="58"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="58"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="58"/>
+      <c r="B36" s="147"/>
+      <c r="C36" s="58"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="58"/>
+      <c r="B37" s="147"/>
+      <c r="C37" s="58"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="58"/>
+      <c r="B38" s="147"/>
+      <c r="C38" s="58"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="58"/>
+      <c r="B39" s="147"/>
+      <c r="C39" s="58"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="58"/>
+      <c r="B40" s="147"/>
+      <c r="C40" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
+  <mergeCells count="37">
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F492E24B-972E-44AA-8E1C-43F16CCC63B2}">
-  <dimension ref="A2:H12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="1.7109375" style="87" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" style="87" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" style="87" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A2" s="86"/>
-      <c r="B2" s="94" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="96"/>
-    </row>
-    <row r="3" spans="1:8" s="87" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-    </row>
-    <row r="4" spans="1:8" ht="25.5">
-      <c r="A4" s="86"/>
-      <c r="B4" s="97" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="97" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="89"/>
-      <c r="H4" s="97" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="87" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-    </row>
-    <row r="6" spans="1:8" ht="38.25">
-      <c r="A6" s="86"/>
-      <c r="B6" s="98" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="98" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="98" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="98" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="87" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A7" s="88"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-    </row>
-    <row r="8" spans="1:8" ht="25.5">
-      <c r="A8" s="86"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="98" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="98" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="87" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A9" s="88"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-    </row>
-    <row r="10" spans="1:8" ht="25.5">
-      <c r="A10" s="86"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="93"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="91"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="86"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="86"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:H2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14985B6A-3B47-4B59-A52E-2C64D685729F}">
-  <dimension ref="B1:C15"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -31106,103 +32405,109 @@
   <sheetData>
     <row r="1" spans="2:3" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="55">
+        <v>43216</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
+      <c r="B3" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
+      <c r="B4" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="79">
-        <v>43216</v>
+      <c r="C4" s="56" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B3" s="78" t="s">
+    <row r="5" spans="2:3" ht="12" customHeight="1">
+      <c r="B5" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C5" s="152" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="12" customHeight="1">
+      <c r="B6" s="108"/>
+      <c r="C6" s="153" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="12" customHeight="1">
+      <c r="B7" s="108"/>
+      <c r="C7" s="154" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="12" customHeight="1">
+      <c r="B8" s="108"/>
+      <c r="C8" s="153" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="12" customHeight="1">
+      <c r="B9" s="108"/>
+      <c r="C9" s="155" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="12" customHeight="1">
+      <c r="B10" s="108"/>
+      <c r="C10" s="153" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" s="65" customFormat="1" ht="12" customHeight="1">
+      <c r="B11" s="151"/>
+      <c r="C11" s="153" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="12" customHeight="1" thickBot="1">
+      <c r="B12" s="109"/>
+      <c r="C12" s="156" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="12" customHeight="1">
+      <c r="B13" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="57" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B4" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="80" t="s">
+    <row r="14" spans="2:3" ht="12" customHeight="1">
+      <c r="B14" s="111"/>
+      <c r="C14" s="52" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="12" customHeight="1">
-      <c r="B5" s="81" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="82" t="s">
+    <row r="15" spans="2:3" ht="12" customHeight="1">
+      <c r="B15" s="111"/>
+      <c r="C15" s="52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="12" customHeight="1">
-      <c r="B6" s="72"/>
-      <c r="C6" s="75" t="s">
+    <row r="16" spans="2:3" ht="12" customHeight="1" thickBot="1">
+      <c r="B16" s="112"/>
+      <c r="C16" s="53" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="12" customHeight="1">
-      <c r="B7" s="72"/>
-      <c r="C7" s="75" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="12" customHeight="1">
-      <c r="B8" s="72"/>
-      <c r="C8" s="75" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="12" customHeight="1">
-      <c r="B9" s="72"/>
-      <c r="C9" s="75" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="12" customHeight="1">
-      <c r="B10" s="72"/>
-      <c r="C10" s="75" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="12" customHeight="1" thickBot="1">
-      <c r="B11" s="83"/>
-      <c r="C11" s="84" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="12" customHeight="1">
-      <c r="B12" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="82" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="12" customHeight="1">
-      <c r="B13" s="73"/>
-      <c r="C13" s="76" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="12" customHeight="1">
-      <c r="B14" s="73"/>
-      <c r="C14" s="76" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="12" customHeight="1" thickBot="1">
-      <c r="B15" s="74"/>
-      <c r="C15" s="77" t="s">
-        <v>83</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31216,7 +32521,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -31248,10 +32553,10 @@
     </row>
     <row r="2" spans="1:13" ht="18.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="48"/>
+      <c r="C2" s="114"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -31271,218 +32576,204 @@
       <c r="E3" s="11">
         <v>2</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="90">
         <v>3</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="87">
         <v>4</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="87">
         <v>5</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="87"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="19" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="84" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+    </row>
+    <row r="6" spans="1:13" ht="12.75" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="58"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A7" s="13"/>
+      <c r="B7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="23">
-        <v>19</v>
-      </c>
-      <c r="E5" s="23">
-        <v>11</v>
-      </c>
-      <c r="F5" s="23">
-        <v>16</v>
-      </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-    </row>
-    <row r="6" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="13"/>
+      <c r="B8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="C8" s="157">
+        <v>200</v>
+      </c>
+      <c r="D8" s="157"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="157"/>
+      <c r="G8" s="158"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="13"/>
+      <c r="B9" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="14"/>
-      <c r="B8" s="21" t="s">
-        <v>30</v>
+      <c r="C9" s="160">
+        <f>$C$8-C$3*($C$8/4)</f>
+        <v>200</v>
       </c>
-      <c r="C8" s="26">
-        <v>17</v>
+      <c r="D9" s="160">
+        <f t="shared" ref="D9:H9" si="0">$C$8-D$3*($C$8/4)</f>
+        <v>150</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="14"/>
-      <c r="B9" s="21" t="s">
-        <v>31</v>
+      <c r="E9" s="160">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
-      <c r="C9" s="38">
-        <f>17-C3*(17/4)</f>
-        <v>17</v>
+      <c r="F9" s="160">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
-      <c r="D9" s="38">
-        <f t="shared" ref="D9:G10" si="0">17-D3*(17/4)</f>
-        <v>12.75</v>
-      </c>
-      <c r="E9" s="38">
-        <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-      <c r="F9" s="38">
-        <f t="shared" si="0"/>
-        <v>4.25</v>
-      </c>
-      <c r="G9" s="38">
+      <c r="G9" s="160">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2"/>
-      <c r="B10" s="39" t="s">
-        <v>32</v>
+      <c r="B10" s="35" t="s">
+        <v>30</v>
       </c>
-      <c r="C10" s="38">
-        <f>17-C3*(17/3)</f>
-        <v>17</v>
+      <c r="C10" s="160">
+        <f>$C$8-C3*($C$8/3)</f>
+        <v>200</v>
       </c>
-      <c r="D10" s="38">
-        <f t="shared" ref="D10:G10" si="1">17-D3*(17/3)</f>
-        <v>11.333333333333332</v>
+      <c r="D10" s="160">
+        <f t="shared" ref="D10:H10" si="1">$C$8-D3*($C$8/3)</f>
+        <v>133.33333333333331</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="160">
         <f t="shared" si="1"/>
-        <v>5.6666666666666661</v>
+        <v>66.666666666666657</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="160">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="38">
-        <f t="shared" si="1"/>
-        <v>-5.6666666666666679</v>
-      </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2"/>
-      <c r="B11" s="39" t="s">
-        <v>33</v>
+      <c r="B11" s="35" t="s">
+        <v>31</v>
       </c>
-      <c r="C11" s="53">
-        <f>17-C$3*(17/5)</f>
-        <v>17</v>
+      <c r="C11" s="160">
+        <f>$C$8-C$3*($C$8/5)</f>
+        <v>200</v>
       </c>
-      <c r="D11" s="53">
-        <f t="shared" ref="D11:H11" si="2">17-D$3*(17/5)</f>
-        <v>13.6</v>
+      <c r="D11" s="160">
+        <f t="shared" ref="D11:H11" si="2">$C$8-D$3*($C$8/5)</f>
+        <v>160</v>
       </c>
-      <c r="E11" s="53">
+      <c r="E11" s="160">
         <f t="shared" si="2"/>
-        <v>10.199999999999999</v>
+        <v>120</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="160">
         <f t="shared" si="2"/>
-        <v>6.8000000000000007</v>
+        <v>80</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="160">
         <f t="shared" si="2"/>
-        <v>3.4000000000000004</v>
+        <v>40</v>
       </c>
-      <c r="H11" s="53">
+      <c r="H11" s="160">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -46336,8 +47627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -46351,7 +47642,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A1" s="41"/>
+      <c r="A1" s="37"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -46374,10 +47665,10 @@
     </row>
     <row r="2" spans="1:20" ht="12.75" customHeight="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="42" t="s">
-        <v>34</v>
+      <c r="B2" s="38" t="s">
+        <v>32</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>

</xml_diff>

<commit_message>
creation base de donnée
</commit_message>
<xml_diff>
--- a/SCRUM/Template suivi projet Fred-Salah.xlsx
+++ b/SCRUM/Template suivi projet Fred-Salah.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagiaire\Desktop\Nouveau dossier\Proxibanque-V3\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A0645E07-686E-4D67-934D-8244B0AD0759}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{89EE1A43-BEE2-49A0-A5E7-3B9109422A54}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8805" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story Mapping" sheetId="6" r:id="rId1"/>
@@ -446,7 +446,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,12 +481,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF3C78D8"/>
         <bgColor rgb="FF3C78D8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -528,6 +522,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9696C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80C8A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDC80"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1216,7 +1246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1367,24 +1397,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1397,13 +1409,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1418,34 +1430,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1454,7 +1466,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1484,81 +1496,6 @@
     <xf numFmtId="3" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1574,20 +1511,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1598,24 +1526,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1625,55 +1535,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1688,12 +1559,189 @@
     <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFDC80"/>
+      <color rgb="FF80C8A0"/>
+      <color rgb="FF9696C8"/>
+      <color rgb="FF7896C8"/>
+      <color rgb="FFFF8080"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2615,6 +2663,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>628650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42033142-77C1-492A-9294-58A9E7ABBE6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3006,231 +3108,231 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1.7109375" style="41" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" style="59" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="53" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="1.7109375" style="59" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" style="53" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" style="59" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" style="53" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="1.7109375" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="38.25" customHeight="1">
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="93" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="95"/>
-      <c r="N2" s="73" t="s">
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="110"/>
+      <c r="N2" s="67" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
+    <row r="3" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:14" ht="25.5">
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="62" t="s">
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="62" t="s">
+      <c r="G4" s="55"/>
+      <c r="H4" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62" t="s">
+      <c r="I4" s="55"/>
+      <c r="J4" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="62" t="s">
+      <c r="K4" s="55"/>
+      <c r="L4" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="62" t="s">
+      <c r="N4" s="56" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
+    <row r="5" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
     </row>
     <row r="6" spans="2:14" ht="38.25">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="111" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="63" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="63" t="s">
+      <c r="G6" s="63"/>
+      <c r="H6" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="69"/>
-      <c r="J6" s="76" t="s">
+      <c r="I6" s="63"/>
+      <c r="J6" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="K6" s="69"/>
-      <c r="L6" s="63" t="s">
+      <c r="K6" s="63"/>
+      <c r="L6" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-    </row>
-    <row r="7" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="B7" s="100"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+    </row>
+    <row r="7" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="B7" s="115"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
     </row>
     <row r="8" spans="2:14" ht="25.5">
-      <c r="B8" s="100"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="63" t="s">
+      <c r="B8" s="115"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="69"/>
-      <c r="J8" s="63" t="s">
+      <c r="I8" s="63"/>
+      <c r="J8" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="70"/>
-      <c r="L8" s="63" t="s">
+      <c r="K8" s="64"/>
+      <c r="L8" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-    </row>
-    <row r="9" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="B9" s="100"/>
-      <c r="D9" s="97"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+    </row>
+    <row r="9" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="B9" s="115"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
     </row>
     <row r="10" spans="2:14" ht="25.5">
-      <c r="B10" s="101"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="64" t="s">
+      <c r="B10" s="116"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
     </row>
     <row r="11" spans="2:14" ht="5.0999999999999996" customHeight="1">
-      <c r="B11" s="72"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="58"/>
+      <c r="B11" s="66"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="52"/>
     </row>
     <row r="12" spans="2:14" ht="25.5">
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="76" t="s">
+      <c r="E12" s="52"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="70"/>
-      <c r="J12" s="76" t="s">
+      <c r="I12" s="64"/>
+      <c r="J12" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="70"/>
-      <c r="L12" s="76" t="s">
+      <c r="K12" s="64"/>
+      <c r="L12" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="M12" s="77"/>
-      <c r="N12" s="75"/>
-    </row>
-    <row r="13" spans="2:14" s="59" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="B13" s="100"/>
-      <c r="D13" s="80"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="69"/>
+    </row>
+    <row r="13" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
+      <c r="B13" s="115"/>
+      <c r="D13" s="74"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
     </row>
     <row r="14" spans="2:14" ht="38.25">
-      <c r="B14" s="101"/>
-      <c r="D14" s="78" t="s">
+      <c r="B14" s="116"/>
+      <c r="D14" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="76" t="s">
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="K14" s="77"/>
-      <c r="L14" s="76" t="s">
+      <c r="K14" s="71"/>
+      <c r="L14" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="M14" s="77"/>
-      <c r="N14" s="76" t="s">
+      <c r="M14" s="71"/>
+      <c r="N14" s="70" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3302,15 +3404,15 @@
     </row>
     <row r="2" spans="1:26" ht="24" customHeight="1">
       <c r="A2" s="4"/>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -3585,10 +3687,10 @@
       <c r="B9" s="19">
         <v>5</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="119" t="s">
+      <c r="D9" s="88" t="s">
         <v>96</v>
       </c>
       <c r="E9" s="24">
@@ -3597,11 +3699,11 @@
       <c r="F9" s="24">
         <v>30</v>
       </c>
-      <c r="G9" s="118" t="s">
+      <c r="G9" s="87" t="s">
         <v>97</v>
       </c>
       <c r="H9" s="28"/>
-      <c r="I9" s="120" t="s">
+      <c r="I9" s="89" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="6"/>
@@ -31386,7 +31488,7 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="40" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="65" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="59" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -31394,35 +31496,35 @@
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="65" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A1" s="65">
+    <row r="1" spans="1:15" s="59" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A1" s="59">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="13.5" thickBot="1">
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="121" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="116" t="s">
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="116" t="s">
+      <c r="I2" s="120"/>
+      <c r="J2" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="117"/>
-      <c r="L2" s="116" t="s">
+      <c r="K2" s="120"/>
+      <c r="L2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="117"/>
-      <c r="N2" s="116" t="s">
+      <c r="M2" s="120"/>
+      <c r="N2" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="117"/>
+      <c r="O2" s="120"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1">
       <c r="B3" s="49" t="s">
@@ -31443,836 +31545,836 @@
       <c r="G3" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="129" t="s">
+      <c r="H3" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="130" t="s">
+      <c r="I3" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="129" t="s">
+      <c r="J3" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="130" t="s">
+      <c r="K3" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="129" t="s">
+      <c r="L3" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="130" t="s">
+      <c r="M3" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="129" t="s">
+      <c r="N3" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="O3" s="130" t="s">
+      <c r="O3" s="96" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="134" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="140">
+      <c r="C4" s="125">
         <v>20</v>
       </c>
-      <c r="D4" s="104">
+      <c r="D4" s="131">
         <f>A$1*C4/'Product Backlog'!I$3</f>
         <v>1.6</v>
       </c>
-      <c r="E4" s="104">
+      <c r="E4" s="131">
         <f>60*D4</f>
         <v>96</v>
       </c>
-      <c r="F4" s="66" t="s">
+      <c r="F4" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G4" s="46">
         <v>15</v>
       </c>
-      <c r="H4" s="137" t="s">
+      <c r="H4" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="144">
+      <c r="I4" s="100">
         <v>15</v>
       </c>
-      <c r="J4" s="66" t="s">
+      <c r="J4" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="125"/>
-      <c r="L4" s="66" t="s">
+      <c r="K4" s="92"/>
+      <c r="L4" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="125"/>
-      <c r="N4" s="66" t="s">
+      <c r="M4" s="92"/>
+      <c r="N4" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="125"/>
+      <c r="O4" s="92"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1">
-      <c r="B5" s="132"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="67" t="s">
+      <c r="B5" s="135"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="47">
         <v>66</v>
       </c>
-      <c r="H5" s="138" t="s">
+      <c r="H5" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="126">
+      <c r="I5" s="93">
         <v>60</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="145">
+      <c r="K5" s="101">
         <v>6</v>
       </c>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="126"/>
-      <c r="N5" s="67" t="s">
+      <c r="M5" s="93"/>
+      <c r="N5" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="126"/>
+      <c r="O5" s="93"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="133"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="68" t="s">
+      <c r="B6" s="136"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="62" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="48">
         <v>15</v>
       </c>
-      <c r="H6" s="139" t="s">
+      <c r="H6" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="128"/>
-      <c r="J6" s="68" t="s">
+      <c r="I6" s="94"/>
+      <c r="J6" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="128"/>
-      <c r="L6" s="68" t="s">
+      <c r="K6" s="94"/>
+      <c r="L6" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="128"/>
-      <c r="N6" s="68" t="s">
+      <c r="M6" s="94"/>
+      <c r="N6" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O6" s="146">
+      <c r="O6" s="102">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="134" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="140">
+      <c r="C7" s="125">
         <v>30</v>
       </c>
-      <c r="D7" s="104">
+      <c r="D7" s="131">
         <f>A$1*C7/'Product Backlog'!I$3</f>
         <v>2.4</v>
       </c>
-      <c r="E7" s="104">
+      <c r="E7" s="131">
         <f t="shared" ref="E7" si="0">60*D7</f>
         <v>144</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G7" s="46">
         <v>15</v>
       </c>
-      <c r="H7" s="137" t="s">
+      <c r="H7" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="144">
+      <c r="I7" s="100">
         <v>15</v>
       </c>
-      <c r="J7" s="66" t="s">
+      <c r="J7" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="125"/>
-      <c r="L7" s="66" t="s">
+      <c r="K7" s="92"/>
+      <c r="L7" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="125"/>
-      <c r="N7" s="66" t="s">
+      <c r="M7" s="92"/>
+      <c r="N7" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="125"/>
+      <c r="O7" s="92"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1">
-      <c r="B8" s="132"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="67" t="s">
+      <c r="B8" s="135"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G8" s="47">
         <v>114</v>
       </c>
-      <c r="H8" s="138" t="s">
+      <c r="H8" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="126">
+      <c r="I8" s="93">
         <v>60</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="145">
+      <c r="K8" s="101">
         <v>54</v>
       </c>
-      <c r="L8" s="67" t="s">
+      <c r="L8" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="126"/>
-      <c r="N8" s="67" t="s">
+      <c r="M8" s="93"/>
+      <c r="N8" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O8" s="126"/>
+      <c r="O8" s="93"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B9" s="133"/>
-      <c r="C9" s="142"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="68" t="s">
+      <c r="B9" s="136"/>
+      <c r="C9" s="127"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="62" t="s">
         <v>58</v>
       </c>
       <c r="G9" s="48">
         <v>15</v>
       </c>
-      <c r="H9" s="139" t="s">
+      <c r="H9" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="128"/>
-      <c r="J9" s="68" t="s">
+      <c r="I9" s="94"/>
+      <c r="J9" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="128"/>
-      <c r="L9" s="68" t="s">
+      <c r="K9" s="94"/>
+      <c r="L9" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="128"/>
-      <c r="N9" s="68" t="s">
+      <c r="M9" s="94"/>
+      <c r="N9" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O9" s="146">
+      <c r="O9" s="102">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1">
-      <c r="B10" s="131" t="s">
+      <c r="B10" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="140">
+      <c r="C10" s="125">
         <v>10</v>
       </c>
-      <c r="D10" s="104">
+      <c r="D10" s="131">
         <f>A$1*C10/'Product Backlog'!I$3</f>
         <v>0.8</v>
       </c>
-      <c r="E10" s="104">
+      <c r="E10" s="131">
         <f t="shared" ref="E10" si="1">60*D10</f>
         <v>48</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G10" s="46">
         <v>15</v>
       </c>
-      <c r="H10" s="137" t="s">
+      <c r="H10" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="144">
+      <c r="I10" s="100">
         <v>15</v>
       </c>
-      <c r="J10" s="66" t="s">
+      <c r="J10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K10" s="125"/>
-      <c r="L10" s="66" t="s">
+      <c r="K10" s="92"/>
+      <c r="L10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="125"/>
-      <c r="N10" s="66" t="s">
+      <c r="M10" s="92"/>
+      <c r="N10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="125"/>
+      <c r="O10" s="92"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1">
-      <c r="B11" s="132"/>
-      <c r="C11" s="141"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="67" t="s">
+      <c r="B11" s="135"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G11" s="47">
         <v>18</v>
       </c>
-      <c r="H11" s="138" t="s">
+      <c r="H11" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="126"/>
-      <c r="J11" s="67" t="s">
+      <c r="I11" s="93"/>
+      <c r="J11" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K11" s="145">
+      <c r="K11" s="101">
         <v>18</v>
       </c>
-      <c r="L11" s="67" t="s">
+      <c r="L11" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="126"/>
-      <c r="N11" s="67" t="s">
+      <c r="M11" s="93"/>
+      <c r="N11" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="126"/>
+      <c r="O11" s="93"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B12" s="133"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="68" t="s">
+      <c r="B12" s="136"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="62" t="s">
         <v>58</v>
       </c>
       <c r="G12" s="48">
         <v>15</v>
       </c>
-      <c r="H12" s="139" t="s">
+      <c r="H12" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="128"/>
-      <c r="J12" s="68" t="s">
+      <c r="I12" s="94"/>
+      <c r="J12" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="128"/>
-      <c r="L12" s="68" t="s">
+      <c r="K12" s="94"/>
+      <c r="L12" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="128"/>
-      <c r="N12" s="68" t="s">
+      <c r="M12" s="94"/>
+      <c r="N12" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O12" s="146">
+      <c r="O12" s="102">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
-      <c r="B13" s="131" t="s">
+      <c r="B13" s="134" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="140">
+      <c r="C13" s="125">
         <v>20</v>
       </c>
-      <c r="D13" s="104">
+      <c r="D13" s="131">
         <f>A$1*C13/'Product Backlog'!I$3</f>
         <v>1.6</v>
       </c>
-      <c r="E13" s="104">
+      <c r="E13" s="131">
         <f t="shared" ref="E13" si="2">60*D13</f>
         <v>96</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G13" s="46">
         <v>15</v>
       </c>
-      <c r="H13" s="137" t="s">
+      <c r="H13" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="144">
+      <c r="I13" s="100">
         <v>15</v>
       </c>
-      <c r="J13" s="66" t="s">
+      <c r="J13" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="125"/>
-      <c r="L13" s="66" t="s">
+      <c r="K13" s="92"/>
+      <c r="L13" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M13" s="125"/>
-      <c r="N13" s="66" t="s">
+      <c r="M13" s="92"/>
+      <c r="N13" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O13" s="125"/>
+      <c r="O13" s="92"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1">
-      <c r="B14" s="132"/>
-      <c r="C14" s="141"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="67" t="s">
+      <c r="B14" s="135"/>
+      <c r="C14" s="126"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G14" s="47">
         <v>66</v>
       </c>
-      <c r="H14" s="138" t="s">
+      <c r="H14" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I14" s="126"/>
-      <c r="J14" s="67" t="s">
+      <c r="I14" s="93"/>
+      <c r="J14" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K14" s="145">
+      <c r="K14" s="101">
         <v>66</v>
       </c>
-      <c r="L14" s="67" t="s">
+      <c r="L14" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M14" s="126"/>
-      <c r="N14" s="67" t="s">
+      <c r="M14" s="93"/>
+      <c r="N14" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O14" s="126"/>
+      <c r="O14" s="93"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B15" s="133"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="68" t="s">
+      <c r="B15" s="136"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="133"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="62" t="s">
         <v>58</v>
       </c>
       <c r="G15" s="48">
         <v>15</v>
       </c>
-      <c r="H15" s="139" t="s">
+      <c r="H15" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="128"/>
-      <c r="J15" s="68" t="s">
+      <c r="I15" s="94"/>
+      <c r="J15" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="128"/>
-      <c r="L15" s="68" t="s">
+      <c r="K15" s="94"/>
+      <c r="L15" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M15" s="128"/>
-      <c r="N15" s="68" t="s">
+      <c r="M15" s="94"/>
+      <c r="N15" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="146">
+      <c r="O15" s="102">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="B16" s="134" t="s">
+      <c r="B16" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="140">
+      <c r="C16" s="125">
         <v>30</v>
       </c>
-      <c r="D16" s="104">
+      <c r="D16" s="131">
         <f>A$1*C16/'Product Backlog'!I$3</f>
         <v>2.4</v>
       </c>
-      <c r="E16" s="104">
+      <c r="E16" s="131">
         <f t="shared" ref="E16" si="3">60*D16</f>
         <v>144</v>
       </c>
-      <c r="F16" s="66" t="s">
+      <c r="F16" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G16" s="46">
         <v>15</v>
       </c>
-      <c r="H16" s="137" t="s">
+      <c r="H16" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="144">
+      <c r="I16" s="100">
         <v>15</v>
       </c>
-      <c r="J16" s="66" t="s">
+      <c r="J16" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="125"/>
-      <c r="L16" s="66" t="s">
+      <c r="K16" s="92"/>
+      <c r="L16" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M16" s="125"/>
-      <c r="N16" s="66" t="s">
+      <c r="M16" s="92"/>
+      <c r="N16" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O16" s="125"/>
+      <c r="O16" s="92"/>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1">
-      <c r="B17" s="135"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="67" t="s">
+      <c r="B17" s="139"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G17" s="47">
         <v>114</v>
       </c>
-      <c r="H17" s="138" t="s">
+      <c r="H17" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I17" s="126"/>
-      <c r="J17" s="67" t="s">
+      <c r="I17" s="93"/>
+      <c r="J17" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="126">
+      <c r="K17" s="93">
         <v>96</v>
       </c>
-      <c r="L17" s="67" t="s">
+      <c r="L17" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M17" s="145">
+      <c r="M17" s="101">
         <v>18</v>
       </c>
-      <c r="N17" s="67" t="s">
+      <c r="N17" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="126"/>
+      <c r="O17" s="93"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B18" s="136"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="68" t="s">
+      <c r="B18" s="140"/>
+      <c r="C18" s="127"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="62" t="s">
         <v>58</v>
       </c>
       <c r="G18" s="48">
         <v>15</v>
       </c>
-      <c r="H18" s="139" t="s">
+      <c r="H18" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I18" s="128"/>
-      <c r="J18" s="68" t="s">
+      <c r="I18" s="94"/>
+      <c r="J18" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="128"/>
-      <c r="L18" s="68" t="s">
+      <c r="K18" s="94"/>
+      <c r="L18" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="128"/>
-      <c r="N18" s="68" t="s">
+      <c r="M18" s="94"/>
+      <c r="N18" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="146">
+      <c r="O18" s="102">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1">
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="140">
+      <c r="C19" s="125">
         <v>20</v>
       </c>
-      <c r="D19" s="104">
+      <c r="D19" s="131">
         <f>A$1*C19/'Product Backlog'!I$3</f>
         <v>1.6</v>
       </c>
-      <c r="E19" s="104">
+      <c r="E19" s="131">
         <f t="shared" ref="E19" si="4">60*D19</f>
         <v>96</v>
       </c>
-      <c r="F19" s="66" t="s">
+      <c r="F19" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G19" s="46">
         <v>15</v>
       </c>
-      <c r="H19" s="137" t="s">
+      <c r="H19" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I19" s="144">
+      <c r="I19" s="100">
         <v>15</v>
       </c>
-      <c r="J19" s="66" t="s">
+      <c r="J19" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K19" s="125"/>
-      <c r="L19" s="66" t="s">
+      <c r="K19" s="92"/>
+      <c r="L19" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M19" s="125"/>
-      <c r="N19" s="66" t="s">
+      <c r="M19" s="92"/>
+      <c r="N19" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="125"/>
+      <c r="O19" s="92"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
-      <c r="B20" s="132"/>
-      <c r="C20" s="141"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="67" t="s">
+      <c r="B20" s="135"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G20" s="47">
         <v>66</v>
       </c>
-      <c r="H20" s="138" t="s">
+      <c r="H20" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I20" s="126"/>
-      <c r="J20" s="67" t="s">
+      <c r="I20" s="93"/>
+      <c r="J20" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="126"/>
-      <c r="L20" s="67" t="s">
+      <c r="K20" s="93"/>
+      <c r="L20" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M20" s="145">
+      <c r="M20" s="101">
         <v>66</v>
       </c>
-      <c r="N20" s="67" t="s">
+      <c r="N20" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O20" s="126"/>
+      <c r="O20" s="93"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B21" s="133"/>
-      <c r="C21" s="142"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="68" t="s">
+      <c r="B21" s="136"/>
+      <c r="C21" s="127"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="62" t="s">
         <v>58</v>
       </c>
       <c r="G21" s="48">
         <v>15</v>
       </c>
-      <c r="H21" s="139" t="s">
+      <c r="H21" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I21" s="128"/>
-      <c r="J21" s="68" t="s">
+      <c r="I21" s="94"/>
+      <c r="J21" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K21" s="128"/>
-      <c r="L21" s="68" t="s">
+      <c r="K21" s="94"/>
+      <c r="L21" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M21" s="128"/>
-      <c r="N21" s="68" t="s">
+      <c r="M21" s="94"/>
+      <c r="N21" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O21" s="146">
+      <c r="O21" s="102">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
-      <c r="B22" s="131" t="s">
+      <c r="B22" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="140">
+      <c r="C22" s="125">
         <v>40</v>
       </c>
-      <c r="D22" s="104">
+      <c r="D22" s="131">
         <f>A$1*C22/'Product Backlog'!I$3</f>
         <v>3.2</v>
       </c>
-      <c r="E22" s="104">
+      <c r="E22" s="131">
         <f t="shared" ref="E22" si="5">60*D22</f>
         <v>192</v>
       </c>
-      <c r="F22" s="66" t="s">
+      <c r="F22" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G22" s="46">
         <v>15</v>
       </c>
-      <c r="H22" s="137" t="s">
+      <c r="H22" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="144">
+      <c r="I22" s="100">
         <v>15</v>
       </c>
-      <c r="J22" s="66" t="s">
+      <c r="J22" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K22" s="125"/>
-      <c r="L22" s="66" t="s">
+      <c r="K22" s="92"/>
+      <c r="L22" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M22" s="125"/>
-      <c r="N22" s="66" t="s">
+      <c r="M22" s="92"/>
+      <c r="N22" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O22" s="125"/>
+      <c r="O22" s="92"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
-      <c r="B23" s="132"/>
-      <c r="C23" s="141"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="67" t="s">
+      <c r="B23" s="135"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G23" s="47">
         <v>162</v>
       </c>
-      <c r="H23" s="138" t="s">
+      <c r="H23" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="126"/>
-      <c r="J23" s="67" t="s">
+      <c r="I23" s="93"/>
+      <c r="J23" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K23" s="126"/>
-      <c r="L23" s="67" t="s">
+      <c r="K23" s="93"/>
+      <c r="L23" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M23" s="126">
+      <c r="M23" s="93">
         <v>156</v>
       </c>
-      <c r="N23" s="67" t="s">
+      <c r="N23" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O23" s="145">
+      <c r="O23" s="101">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B24" s="133"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="121" t="s">
+      <c r="B24" s="136"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="122">
+      <c r="G24" s="91">
         <v>15</v>
       </c>
-      <c r="H24" s="139" t="s">
+      <c r="H24" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="128"/>
-      <c r="J24" s="68" t="s">
+      <c r="I24" s="94"/>
+      <c r="J24" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K24" s="128"/>
-      <c r="L24" s="68" t="s">
+      <c r="K24" s="94"/>
+      <c r="L24" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M24" s="128"/>
-      <c r="N24" s="68" t="s">
+      <c r="M24" s="94"/>
+      <c r="N24" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O24" s="146">
+      <c r="O24" s="102">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
-      <c r="B25" s="148" t="s">
+      <c r="B25" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="140">
+      <c r="C25" s="125">
         <v>30</v>
       </c>
-      <c r="D25" s="124">
+      <c r="D25" s="128">
         <f>A$1*C25/'Product Backlog'!I$3</f>
         <v>2.4</v>
       </c>
-      <c r="E25" s="104">
+      <c r="E25" s="131">
         <f t="shared" ref="E25" si="6">60*D25</f>
         <v>144</v>
       </c>
-      <c r="F25" s="66" t="s">
+      <c r="F25" s="60" t="s">
         <v>56</v>
       </c>
       <c r="G25" s="46">
         <v>15</v>
       </c>
-      <c r="H25" s="137" t="s">
+      <c r="H25" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="144">
+      <c r="I25" s="100">
         <v>15</v>
       </c>
-      <c r="J25" s="66" t="s">
+      <c r="J25" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="K25" s="125"/>
-      <c r="L25" s="66" t="s">
+      <c r="K25" s="92"/>
+      <c r="L25" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="M25" s="125"/>
-      <c r="N25" s="66" t="s">
+      <c r="M25" s="92"/>
+      <c r="N25" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="O25" s="125"/>
+      <c r="O25" s="92"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
-      <c r="B26" s="149"/>
-      <c r="C26" s="141"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="67" t="s">
+      <c r="B26" s="123"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="61" t="s">
         <v>57</v>
       </c>
       <c r="G26" s="47">
         <v>114</v>
       </c>
-      <c r="H26" s="138" t="s">
+      <c r="H26" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="I26" s="126"/>
-      <c r="J26" s="67" t="s">
+      <c r="I26" s="93"/>
+      <c r="J26" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="K26" s="126"/>
-      <c r="L26" s="67" t="s">
+      <c r="K26" s="93"/>
+      <c r="L26" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="M26" s="126"/>
-      <c r="N26" s="67" t="s">
+      <c r="M26" s="93"/>
+      <c r="N26" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O26" s="145">
+      <c r="O26" s="101">
         <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B27" s="150"/>
-      <c r="C27" s="142"/>
-      <c r="D27" s="127"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="68" t="s">
+      <c r="B27" s="124"/>
+      <c r="C27" s="127"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="62" t="s">
         <v>58</v>
       </c>
       <c r="G27" s="48">
         <v>15</v>
       </c>
-      <c r="H27" s="139" t="s">
+      <c r="H27" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="I27" s="128"/>
-      <c r="J27" s="68" t="s">
+      <c r="I27" s="94"/>
+      <c r="J27" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="K27" s="128"/>
-      <c r="L27" s="68" t="s">
+      <c r="K27" s="94"/>
+      <c r="L27" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="M27" s="128"/>
-      <c r="N27" s="68" t="s">
+      <c r="M27" s="94"/>
+      <c r="N27" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="O27" s="146">
+      <c r="O27" s="102">
         <v>15</v>
       </c>
     </row>
@@ -32281,76 +32383,87 @@
         <f>SUM(I4:I27)</f>
         <v>240</v>
       </c>
-      <c r="K30" s="65">
+      <c r="K30" s="59">
         <f>SUM(K4:K27)</f>
         <v>240</v>
       </c>
-      <c r="M30" s="65">
+      <c r="M30" s="59">
         <f>SUM(M4:M27)</f>
         <v>240</v>
       </c>
-      <c r="O30" s="65">
+      <c r="O30" s="59">
         <f>SUM(O4:O27)</f>
         <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="58"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="58"/>
-      <c r="B32" s="147"/>
-      <c r="C32" s="58"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="52"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="58"/>
-      <c r="B33" s="147"/>
-      <c r="C33" s="58"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="52"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="58"/>
-      <c r="B34" s="147"/>
-      <c r="C34" s="58"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="52"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="58"/>
-      <c r="B35" s="147"/>
-      <c r="C35" s="58"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="52"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="58"/>
-      <c r="B36" s="147"/>
-      <c r="C36" s="58"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="52"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="58"/>
-      <c r="B37" s="147"/>
-      <c r="C37" s="58"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="103"/>
+      <c r="C37" s="52"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="58"/>
-      <c r="B38" s="147"/>
-      <c r="C38" s="58"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="103"/>
+      <c r="C38" s="52"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="58"/>
-      <c r="B39" s="147"/>
-      <c r="C39" s="58"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="52"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="58"/>
-      <c r="B40" s="147"/>
-      <c r="C40" s="58"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="D25:D27"/>
@@ -32367,22 +32480,11 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32393,8 +32495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14985B6A-3B47-4B59-A52E-2C64D685729F}">
   <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -32405,102 +32507,102 @@
   <sheetData>
     <row r="1" spans="2:3" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="155" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="156">
         <v>43216</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="157" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="158" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="12" customHeight="1">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="149" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="152" t="s">
+      <c r="C5" s="159" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="12" customHeight="1">
-      <c r="B6" s="108"/>
-      <c r="C6" s="153" t="s">
+      <c r="B6" s="150"/>
+      <c r="C6" s="160" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="12" customHeight="1">
-      <c r="B7" s="108"/>
-      <c r="C7" s="154" t="s">
+      <c r="B7" s="150"/>
+      <c r="C7" s="161" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="12" customHeight="1">
-      <c r="B8" s="108"/>
-      <c r="C8" s="153" t="s">
+      <c r="B8" s="150"/>
+      <c r="C8" s="160" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="12" customHeight="1">
-      <c r="B9" s="108"/>
-      <c r="C9" s="155" t="s">
+      <c r="B9" s="150"/>
+      <c r="C9" s="162" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="12" customHeight="1">
-      <c r="B10" s="108"/>
-      <c r="C10" s="153" t="s">
+      <c r="B10" s="150"/>
+      <c r="C10" s="160" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:3" s="65" customFormat="1" ht="12" customHeight="1">
+    <row r="11" spans="2:3" s="59" customFormat="1" ht="12" customHeight="1">
       <c r="B11" s="151"/>
-      <c r="C11" s="153" t="s">
+      <c r="C11" s="160" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="12" customHeight="1" thickBot="1">
-      <c r="B12" s="109"/>
-      <c r="C12" s="156" t="s">
+      <c r="B12" s="152"/>
+      <c r="C12" s="163" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="12" customHeight="1">
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="143" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="12" customHeight="1">
-      <c r="B14" s="111"/>
-      <c r="C14" s="52" t="s">
+      <c r="B14" s="147"/>
+      <c r="C14" s="144" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="12" customHeight="1">
-      <c r="B15" s="111"/>
-      <c r="C15" s="52" t="s">
+      <c r="B15" s="147"/>
+      <c r="C15" s="144" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="12" customHeight="1" thickBot="1">
-      <c r="B16" s="112"/>
-      <c r="C16" s="53" t="s">
+      <c r="B16" s="148"/>
+      <c r="C16" s="145" t="s">
         <v>74</v>
       </c>
     </row>
@@ -32510,6 +32612,7 @@
     <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -32553,10 +32656,10 @@
     </row>
     <row r="2" spans="1:13" ht="18.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="114"/>
+      <c r="C2" s="142"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -32576,16 +32679,16 @@
       <c r="E3" s="11">
         <v>2</v>
       </c>
-      <c r="F3" s="90">
+      <c r="F3" s="84">
         <v>3</v>
       </c>
-      <c r="G3" s="87">
+      <c r="G3" s="81">
         <v>4</v>
       </c>
-      <c r="H3" s="87">
+      <c r="H3" s="81">
         <v>5</v>
       </c>
-      <c r="I3" s="87"/>
+      <c r="I3" s="81"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="13"/>
@@ -32596,19 +32699,19 @@
       <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="84" t="s">
+      <c r="G4" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="84" t="s">
+      <c r="H4" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I4" s="78" t="s">
         <v>18</v>
       </c>
     </row>
@@ -32619,11 +32722,11 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
       <c r="J5" s="26"/>
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
@@ -32634,11 +32737,11 @@
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
       <c r="E6" s="31"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="58"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="52"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="13"/>
@@ -32657,59 +32760,59 @@
       <c r="F7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="82" t="s">
+      <c r="G7" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="91" t="s">
+      <c r="H7" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="13"/>
       <c r="B8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="157">
+      <c r="C8" s="104">
         <v>200</v>
       </c>
-      <c r="D8" s="157"/>
-      <c r="E8" s="157"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="158"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="13"/>
       <c r="B9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="160">
+      <c r="C9" s="107">
         <f>$C$8-C$3*($C$8/4)</f>
         <v>200</v>
       </c>
-      <c r="D9" s="160">
-        <f t="shared" ref="D9:H9" si="0">$C$8-D$3*($C$8/4)</f>
+      <c r="D9" s="107">
+        <f t="shared" ref="D9:G9" si="0">$C$8-D$3*($C$8/4)</f>
         <v>150</v>
       </c>
-      <c r="E9" s="160">
+      <c r="E9" s="107">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F9" s="160">
+      <c r="F9" s="107">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G9" s="160">
+      <c r="G9" s="107">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="160"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -32719,26 +32822,26 @@
       <c r="B10" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="160">
+      <c r="C10" s="107">
         <f>$C$8-C3*($C$8/3)</f>
         <v>200</v>
       </c>
-      <c r="D10" s="160">
-        <f t="shared" ref="D10:H10" si="1">$C$8-D3*($C$8/3)</f>
+      <c r="D10" s="107">
+        <f t="shared" ref="D10:F10" si="1">$C$8-D3*($C$8/3)</f>
         <v>133.33333333333331</v>
       </c>
-      <c r="E10" s="160">
+      <c r="E10" s="107">
         <f t="shared" si="1"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="F10" s="160">
+      <c r="F10" s="107">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="160"/>
-      <c r="H10" s="160"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -32748,32 +32851,32 @@
       <c r="B11" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="160">
+      <c r="C11" s="107">
         <f>$C$8-C$3*($C$8/5)</f>
         <v>200</v>
       </c>
-      <c r="D11" s="160">
+      <c r="D11" s="107">
         <f t="shared" ref="D11:H11" si="2">$C$8-D$3*($C$8/5)</f>
         <v>160</v>
       </c>
-      <c r="E11" s="160">
+      <c r="E11" s="107">
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="F11" s="160">
+      <c r="F11" s="107">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="G11" s="160">
+      <c r="G11" s="107">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="H11" s="160">
+      <c r="H11" s="107">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -47627,7 +47730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
suite travail sur l'ecran de connexion et sur l'affichage des clients du conseiller + tentative d'ajout d'une fonctionalite de modification d'un client
</commit_message>
<xml_diff>
--- a/SCRUM/Template suivi projet Fred-Salah.xlsx
+++ b/SCRUM/Template suivi projet Fred-Salah.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagiaire\Desktop\Nouveau dossier\Proxibanque-V3\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{89EE1A43-BEE2-49A0-A5E7-3B9109422A54}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FE6E2F34-9988-4D8B-8D74-5AB674A5DBEF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8805" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story Mapping" sheetId="6" r:id="rId1"/>
@@ -1559,6 +1559,48 @@
     <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1658,30 +1700,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1694,38 +1712,20 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1825,9 +1825,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
+              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$G$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -1843,20 +1843,29 @@
                 <c:pt idx="4">
                   <c:v>Fin S4</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Fin S5</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Suivi Release &amp; Vélocité'!$C$8:$H$8</c:f>
+              <c:f>'Suivi Release &amp; Vélocité'!$C$8:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1894,9 +1903,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
+              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$G$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -1911,9 +1920,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fin S4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Fin S5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1975,9 +1981,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
+              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$G$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -1992,9 +1998,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fin S4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Fin S5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2053,9 +2056,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$J$7</c:f>
+              <c:f>'Suivi Release &amp; Vélocité'!$C$7:$G$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Démarrage</c:v>
                 </c:pt>
@@ -2070,9 +2073,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fin S4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Fin S5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2717,6 +2717,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>628650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F62A55FC-3CEA-469F-8BDC-114DBB1797E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>628650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E7F96D6-06D9-4ABE-A4D4-A93AF4C479C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3121,15 +3229,15 @@
     <row r="2" spans="2:14" ht="38.25" customHeight="1">
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="110"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="124"/>
       <c r="N2" s="67" t="s">
         <v>82</v>
       </c>
@@ -3179,10 +3287,10 @@
       <c r="L5" s="55"/>
     </row>
     <row r="6" spans="2:14" ht="38.25">
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="125" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="52"/>
@@ -3205,8 +3313,8 @@
       <c r="N6" s="69"/>
     </row>
     <row r="7" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="B7" s="115"/>
-      <c r="D7" s="112"/>
+      <c r="B7" s="129"/>
+      <c r="D7" s="126"/>
       <c r="E7" s="54"/>
       <c r="F7" s="63"/>
       <c r="G7" s="63"/>
@@ -3219,8 +3327,8 @@
       <c r="N7" s="69"/>
     </row>
     <row r="8" spans="2:14" ht="25.5">
-      <c r="B8" s="115"/>
-      <c r="D8" s="112"/>
+      <c r="B8" s="129"/>
+      <c r="D8" s="126"/>
       <c r="E8" s="52"/>
       <c r="F8" s="64"/>
       <c r="G8" s="64"/>
@@ -3239,8 +3347,8 @@
       <c r="N8" s="69"/>
     </row>
     <row r="9" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="B9" s="115"/>
-      <c r="D9" s="112"/>
+      <c r="B9" s="129"/>
+      <c r="D9" s="126"/>
       <c r="E9" s="54"/>
       <c r="F9" s="63"/>
       <c r="G9" s="63"/>
@@ -3253,8 +3361,8 @@
       <c r="N9" s="69"/>
     </row>
     <row r="10" spans="2:14" ht="25.5">
-      <c r="B10" s="116"/>
-      <c r="D10" s="113"/>
+      <c r="B10" s="130"/>
+      <c r="D10" s="127"/>
       <c r="E10" s="52"/>
       <c r="F10" s="64"/>
       <c r="G10" s="64"/>
@@ -3281,7 +3389,7 @@
       <c r="L11" s="52"/>
     </row>
     <row r="12" spans="2:14" ht="25.5">
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="128" t="s">
         <v>92</v>
       </c>
       <c r="D12" s="75" t="s">
@@ -3305,7 +3413,7 @@
       <c r="N12" s="69"/>
     </row>
     <row r="13" spans="2:14" s="53" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="B13" s="115"/>
+      <c r="B13" s="129"/>
       <c r="D13" s="74"/>
       <c r="H13" s="73"/>
       <c r="I13" s="73"/>
@@ -3316,7 +3424,7 @@
       <c r="N13" s="73"/>
     </row>
     <row r="14" spans="2:14" ht="38.25">
-      <c r="B14" s="116"/>
+      <c r="B14" s="130"/>
       <c r="D14" s="72" t="s">
         <v>91</v>
       </c>
@@ -3404,15 +3512,15 @@
     </row>
     <row r="2" spans="1:26" ht="24" customHeight="1">
       <c r="A2" s="4"/>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -31480,7 +31588,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B27"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -31502,29 +31610,29 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="13.5" thickBot="1">
-      <c r="C2" s="121" t="s">
+      <c r="C2" s="135" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="119" t="s">
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="120"/>
-      <c r="J2" s="119" t="s">
+      <c r="I2" s="134"/>
+      <c r="J2" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="120"/>
-      <c r="L2" s="119" t="s">
+      <c r="K2" s="134"/>
+      <c r="L2" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="120"/>
-      <c r="N2" s="119" t="s">
+      <c r="M2" s="134"/>
+      <c r="N2" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="120"/>
+      <c r="O2" s="134"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1">
       <c r="B3" s="49" t="s">
@@ -31571,17 +31679,17 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1">
-      <c r="B4" s="134" t="s">
+      <c r="B4" s="148" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="125">
+      <c r="C4" s="139">
         <v>20</v>
       </c>
-      <c r="D4" s="131">
+      <c r="D4" s="145">
         <f>A$1*C4/'Product Backlog'!I$3</f>
         <v>1.6</v>
       </c>
-      <c r="E4" s="131">
+      <c r="E4" s="145">
         <f>60*D4</f>
         <v>96</v>
       </c>
@@ -31611,10 +31719,10 @@
       <c r="O4" s="92"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1">
-      <c r="B5" s="135"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
+      <c r="B5" s="149"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
       <c r="F5" s="61" t="s">
         <v>57</v>
       </c>
@@ -31643,10 +31751,10 @@
       <c r="O5" s="93"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="136"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
+      <c r="B6" s="150"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="147"/>
       <c r="F6" s="62" t="s">
         <v>58</v>
       </c>
@@ -31673,17 +31781,17 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="125">
+      <c r="C7" s="139">
         <v>30</v>
       </c>
-      <c r="D7" s="131">
+      <c r="D7" s="145">
         <f>A$1*C7/'Product Backlog'!I$3</f>
         <v>2.4</v>
       </c>
-      <c r="E7" s="131">
+      <c r="E7" s="145">
         <f t="shared" ref="E7" si="0">60*D7</f>
         <v>144</v>
       </c>
@@ -31713,10 +31821,10 @@
       <c r="O7" s="92"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1">
-      <c r="B8" s="135"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
+      <c r="B8" s="149"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="146"/>
       <c r="F8" s="61" t="s">
         <v>57</v>
       </c>
@@ -31745,10 +31853,10 @@
       <c r="O8" s="93"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B9" s="136"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
+      <c r="B9" s="150"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="147"/>
       <c r="F9" s="62" t="s">
         <v>58</v>
       </c>
@@ -31775,17 +31883,17 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1">
-      <c r="B10" s="134" t="s">
+      <c r="B10" s="148" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="125">
+      <c r="C10" s="139">
         <v>10</v>
       </c>
-      <c r="D10" s="131">
+      <c r="D10" s="145">
         <f>A$1*C10/'Product Backlog'!I$3</f>
         <v>0.8</v>
       </c>
-      <c r="E10" s="131">
+      <c r="E10" s="145">
         <f t="shared" ref="E10" si="1">60*D10</f>
         <v>48</v>
       </c>
@@ -31815,10 +31923,10 @@
       <c r="O10" s="92"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1">
-      <c r="B11" s="135"/>
-      <c r="C11" s="126"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="132"/>
+      <c r="B11" s="149"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="146"/>
+      <c r="E11" s="146"/>
       <c r="F11" s="61" t="s">
         <v>57</v>
       </c>
@@ -31845,10 +31953,10 @@
       <c r="O11" s="93"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B12" s="136"/>
-      <c r="C12" s="127"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
+      <c r="B12" s="150"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
       <c r="F12" s="62" t="s">
         <v>58</v>
       </c>
@@ -31875,17 +31983,17 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="148" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="125">
+      <c r="C13" s="139">
         <v>20</v>
       </c>
-      <c r="D13" s="131">
+      <c r="D13" s="145">
         <f>A$1*C13/'Product Backlog'!I$3</f>
         <v>1.6</v>
       </c>
-      <c r="E13" s="131">
+      <c r="E13" s="145">
         <f t="shared" ref="E13" si="2">60*D13</f>
         <v>96</v>
       </c>
@@ -31915,10 +32023,10 @@
       <c r="O13" s="92"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1">
-      <c r="B14" s="135"/>
-      <c r="C14" s="126"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="132"/>
+      <c r="B14" s="149"/>
+      <c r="C14" s="140"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="146"/>
       <c r="F14" s="61" t="s">
         <v>57</v>
       </c>
@@ -31945,10 +32053,10 @@
       <c r="O14" s="93"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B15" s="136"/>
-      <c r="C15" s="127"/>
-      <c r="D15" s="133"/>
-      <c r="E15" s="133"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="147"/>
       <c r="F15" s="62" t="s">
         <v>58</v>
       </c>
@@ -31975,17 +32083,17 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="125">
+      <c r="C16" s="139">
         <v>30</v>
       </c>
-      <c r="D16" s="131">
+      <c r="D16" s="145">
         <f>A$1*C16/'Product Backlog'!I$3</f>
         <v>2.4</v>
       </c>
-      <c r="E16" s="131">
+      <c r="E16" s="145">
         <f t="shared" ref="E16" si="3">60*D16</f>
         <v>144</v>
       </c>
@@ -32015,10 +32123,10 @@
       <c r="O16" s="92"/>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1">
-      <c r="B17" s="139"/>
-      <c r="C17" s="126"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="132"/>
+      <c r="B17" s="153"/>
+      <c r="C17" s="140"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
       <c r="F17" s="61" t="s">
         <v>57</v>
       </c>
@@ -32047,10 +32155,10 @@
       <c r="O17" s="93"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B18" s="140"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="133"/>
+      <c r="B18" s="154"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="147"/>
       <c r="F18" s="62" t="s">
         <v>58</v>
       </c>
@@ -32077,17 +32185,17 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1">
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="148" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="125">
+      <c r="C19" s="139">
         <v>20</v>
       </c>
-      <c r="D19" s="131">
+      <c r="D19" s="145">
         <f>A$1*C19/'Product Backlog'!I$3</f>
         <v>1.6</v>
       </c>
-      <c r="E19" s="131">
+      <c r="E19" s="145">
         <f t="shared" ref="E19" si="4">60*D19</f>
         <v>96</v>
       </c>
@@ -32117,10 +32225,10 @@
       <c r="O19" s="92"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
-      <c r="B20" s="135"/>
-      <c r="C20" s="126"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="132"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="140"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="146"/>
       <c r="F20" s="61" t="s">
         <v>57</v>
       </c>
@@ -32147,10 +32255,10 @@
       <c r="O20" s="93"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B21" s="136"/>
-      <c r="C21" s="127"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="133"/>
+      <c r="B21" s="150"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="147"/>
       <c r="F21" s="62" t="s">
         <v>58</v>
       </c>
@@ -32177,17 +32285,17 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
-      <c r="B22" s="134" t="s">
+      <c r="B22" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="125">
+      <c r="C22" s="139">
         <v>40</v>
       </c>
-      <c r="D22" s="131">
+      <c r="D22" s="145">
         <f>A$1*C22/'Product Backlog'!I$3</f>
         <v>3.2</v>
       </c>
-      <c r="E22" s="131">
+      <c r="E22" s="145">
         <f t="shared" ref="E22" si="5">60*D22</f>
         <v>192</v>
       </c>
@@ -32217,10 +32325,10 @@
       <c r="O22" s="92"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
-      <c r="B23" s="135"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="132"/>
-      <c r="E23" s="132"/>
+      <c r="B23" s="149"/>
+      <c r="C23" s="140"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="146"/>
       <c r="F23" s="61" t="s">
         <v>57</v>
       </c>
@@ -32249,10 +32357,10 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B24" s="136"/>
-      <c r="C24" s="137"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="133"/>
+      <c r="B24" s="150"/>
+      <c r="C24" s="151"/>
+      <c r="D24" s="146"/>
+      <c r="E24" s="147"/>
       <c r="F24" s="90" t="s">
         <v>58</v>
       </c>
@@ -32279,17 +32387,17 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
-      <c r="B25" s="122" t="s">
+      <c r="B25" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="125">
+      <c r="C25" s="139">
         <v>30</v>
       </c>
-      <c r="D25" s="128">
+      <c r="D25" s="142">
         <f>A$1*C25/'Product Backlog'!I$3</f>
         <v>2.4</v>
       </c>
-      <c r="E25" s="131">
+      <c r="E25" s="145">
         <f t="shared" ref="E25" si="6">60*D25</f>
         <v>144</v>
       </c>
@@ -32319,10 +32427,10 @@
       <c r="O25" s="92"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
-      <c r="B26" s="123"/>
-      <c r="C26" s="126"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="132"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="143"/>
+      <c r="E26" s="146"/>
       <c r="F26" s="61" t="s">
         <v>57</v>
       </c>
@@ -32349,10 +32457,10 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B27" s="124"/>
-      <c r="C27" s="127"/>
-      <c r="D27" s="130"/>
-      <c r="E27" s="133"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="147"/>
       <c r="F27" s="62" t="s">
         <v>58</v>
       </c>
@@ -32495,7 +32603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14985B6A-3B47-4B59-A52E-2C64D685729F}">
   <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -32507,102 +32615,102 @@
   <sheetData>
     <row r="1" spans="2:3" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="156">
+      <c r="C2" s="114">
         <v>43216</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="157" t="s">
+      <c r="C3" s="115" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="27.95" customHeight="1" thickBot="1">
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="116" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="12" customHeight="1">
-      <c r="B5" s="149" t="s">
+      <c r="B5" s="155" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="117" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="12" customHeight="1">
-      <c r="B6" s="150"/>
-      <c r="C6" s="160" t="s">
+      <c r="B6" s="156"/>
+      <c r="C6" s="118" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="12" customHeight="1">
-      <c r="B7" s="150"/>
-      <c r="C7" s="161" t="s">
+      <c r="B7" s="156"/>
+      <c r="C7" s="119" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="12" customHeight="1">
-      <c r="B8" s="150"/>
-      <c r="C8" s="160" t="s">
+      <c r="B8" s="156"/>
+      <c r="C8" s="118" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="12" customHeight="1">
-      <c r="B9" s="150"/>
-      <c r="C9" s="162" t="s">
+      <c r="B9" s="156"/>
+      <c r="C9" s="120" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="12" customHeight="1">
-      <c r="B10" s="150"/>
-      <c r="C10" s="160" t="s">
+      <c r="B10" s="156"/>
+      <c r="C10" s="118" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:3" s="59" customFormat="1" ht="12" customHeight="1">
-      <c r="B11" s="151"/>
-      <c r="C11" s="160" t="s">
+      <c r="B11" s="157"/>
+      <c r="C11" s="118" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="12" customHeight="1" thickBot="1">
-      <c r="B12" s="152"/>
-      <c r="C12" s="163" t="s">
+      <c r="B12" s="158"/>
+      <c r="C12" s="121" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="12" customHeight="1">
-      <c r="B13" s="146" t="s">
+      <c r="B13" s="159" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="108" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="12" customHeight="1">
-      <c r="B14" s="147"/>
-      <c r="C14" s="144" t="s">
+      <c r="B14" s="160"/>
+      <c r="C14" s="109" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="12" customHeight="1">
-      <c r="B15" s="147"/>
-      <c r="C15" s="144" t="s">
+      <c r="B15" s="160"/>
+      <c r="C15" s="109" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="12" customHeight="1" thickBot="1">
-      <c r="B16" s="148"/>
-      <c r="C16" s="145" t="s">
+      <c r="B16" s="161"/>
+      <c r="C16" s="110" t="s">
         <v>74</v>
       </c>
     </row>
@@ -32624,7 +32732,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -32656,10 +32764,10 @@
     </row>
     <row r="2" spans="1:13" ht="18.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="142"/>
+      <c r="C2" s="163"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -32777,10 +32885,18 @@
       <c r="C8" s="104">
         <v>200</v>
       </c>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="105"/>
+      <c r="D8" s="104">
+        <v>180</v>
+      </c>
+      <c r="E8" s="104">
+        <v>160</v>
+      </c>
+      <c r="F8" s="104">
+        <v>140</v>
+      </c>
+      <c r="G8" s="105">
+        <v>120</v>
+      </c>
       <c r="H8" s="106"/>
       <c r="I8" s="79"/>
       <c r="J8" s="79"/>
@@ -47730,8 +47846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>